<commit_message>
final script/data/plots for RWYs with labels
</commit_message>
<xml_diff>
--- a/data-ad-charts/APT_BBOX.xlsx
+++ b/data-ad-charts/APT_BBOX.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkoelle\RProjects\dev-flexdashboard\data-ad-charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spi\repos\pru-apt-dashboards\data-ad-charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13656"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="630">
   <si>
     <t>AIRPORT</t>
   </si>
@@ -1915,6 +1915,12 @@
   </si>
   <si>
     <t>29.284744,40.885421,29.327917,40.914356</t>
+  </si>
+  <si>
+    <t>12.257481,57.644849,12.310181,57.680844</t>
+  </si>
+  <si>
+    <t>25.260916,54.613734,25.306835,54.656407</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2115,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:D94" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B1:D94"/>
   <tableColumns count="3">
     <tableColumn id="1" name="AIRPORT" dataDxfId="2"/>
     <tableColumn id="3" name="APT_NAME" dataDxfId="1"/>
@@ -2386,18 +2391,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>215</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2425,7 +2430,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -2453,7 +2458,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -2467,7 +2472,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -2481,7 +2486,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -2495,7 +2500,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2509,7 +2514,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -2523,7 +2528,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2542,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -2551,7 +2556,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -2593,7 +2598,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2607,7 +2612,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
@@ -2621,7 +2626,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -2635,7 +2640,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -2649,7 +2654,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
@@ -2663,7 +2668,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
@@ -2677,7 +2682,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
@@ -2691,7 +2696,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>44</v>
       </c>
@@ -2705,7 +2710,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
@@ -2719,7 +2724,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>44</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>44</v>
       </c>
@@ -2747,7 +2752,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>44</v>
       </c>
@@ -2761,7 +2766,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>44</v>
       </c>
@@ -2775,7 +2780,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
@@ -2789,7 +2794,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>44</v>
       </c>
@@ -2803,7 +2808,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>44</v>
       </c>
@@ -2817,7 +2822,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>44</v>
       </c>
@@ -2831,7 +2836,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>44</v>
       </c>
@@ -2845,7 +2850,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>69</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>72</v>
       </c>
@@ -2873,7 +2878,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>72</v>
       </c>
@@ -2887,7 +2892,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>77</v>
       </c>
@@ -2901,7 +2906,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>80</v>
       </c>
@@ -2915,7 +2920,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>82</v>
       </c>
@@ -2929,7 +2934,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>82</v>
       </c>
@@ -2943,7 +2948,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>82</v>
       </c>
@@ -2957,7 +2962,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>82</v>
       </c>
@@ -2971,7 +2976,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>91</v>
       </c>
@@ -2985,7 +2990,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>94</v>
       </c>
@@ -2995,11 +3000,11 @@
       <c r="C43" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>94</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>99</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>102</v>
       </c>
@@ -3037,11 +3042,11 @@
       <c r="C46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>105</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>105</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>105</v>
       </c>
@@ -3083,7 +3088,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>105</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>105</v>
       </c>
@@ -3111,7 +3116,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>116</v>
       </c>
@@ -3125,7 +3130,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>119</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>122</v>
       </c>
@@ -3153,7 +3158,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>105</v>
       </c>
@@ -3167,7 +3172,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>105</v>
       </c>
@@ -3181,7 +3186,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>105</v>
       </c>
@@ -3195,7 +3200,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>105</v>
       </c>
@@ -3209,7 +3214,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>105</v>
       </c>
@@ -3223,7 +3228,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>105</v>
       </c>
@@ -3237,7 +3242,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>105</v>
       </c>
@@ -3251,7 +3256,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>105</v>
       </c>
@@ -3265,7 +3270,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>105</v>
       </c>
@@ -3279,7 +3284,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>143</v>
       </c>
@@ -3293,7 +3298,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>143</v>
       </c>
@@ -3307,7 +3312,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>143</v>
       </c>
@@ -3321,7 +3326,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>143</v>
       </c>
@@ -3335,7 +3340,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>143</v>
       </c>
@@ -3349,7 +3354,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>143</v>
       </c>
@@ -3363,7 +3368,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>143</v>
       </c>
@@ -3377,7 +3382,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>158</v>
       </c>
@@ -3391,7 +3396,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>161</v>
       </c>
@@ -3405,7 +3410,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>164</v>
       </c>
@@ -3419,7 +3424,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>164</v>
       </c>
@@ -3433,7 +3438,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>164</v>
       </c>
@@ -3447,7 +3452,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>164</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>164</v>
       </c>
@@ -3475,7 +3480,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>164</v>
       </c>
@@ -3489,7 +3494,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>164</v>
       </c>
@@ -3503,7 +3508,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>164</v>
       </c>
@@ -3517,7 +3522,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>164</v>
       </c>
@@ -3531,7 +3536,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>164</v>
       </c>
@@ -3545,7 +3550,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>185</v>
       </c>
@@ -3559,7 +3564,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>188</v>
       </c>
@@ -3573,7 +3578,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>191</v>
       </c>
@@ -3587,7 +3592,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>193</v>
       </c>
@@ -3601,7 +3606,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>196</v>
       </c>
@@ -3615,7 +3620,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>196</v>
       </c>
@@ -3629,7 +3634,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>201</v>
       </c>
@@ -3643,7 +3648,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>204</v>
       </c>
@@ -3657,7 +3662,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>204</v>
       </c>
@@ -3671,7 +3676,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>209</v>
       </c>
@@ -3685,7 +3690,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>7</v>
       </c>
@@ -3699,7 +3704,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>196</v>
       </c>
@@ -3731,15 +3736,15 @@
       <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>215</v>
       </c>
@@ -3753,7 +3758,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>193</v>
       </c>
@@ -3767,7 +3772,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>193</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>193</v>
       </c>
@@ -3795,7 +3800,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>193</v>
       </c>
@@ -3809,7 +3814,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>193</v>
       </c>
@@ -3823,7 +3828,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -3837,7 +3842,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3851,7 +3856,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -3865,7 +3870,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>119</v>
       </c>
@@ -3879,7 +3884,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>188</v>
       </c>
@@ -3893,7 +3898,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>188</v>
       </c>
@@ -3907,7 +3912,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>188</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -3935,7 +3940,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>143</v>
       </c>
@@ -3949,7 +3954,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>143</v>
       </c>
@@ -3963,7 +3968,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>143</v>
       </c>
@@ -3977,7 +3982,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>143</v>
       </c>
@@ -3991,7 +3996,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>143</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>143</v>
       </c>
@@ -4019,7 +4024,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>143</v>
       </c>
@@ -4033,7 +4038,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -4047,7 +4052,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>143</v>
       </c>
@@ -4061,7 +4066,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>143</v>
       </c>
@@ -4075,7 +4080,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>143</v>
       </c>
@@ -4089,7 +4094,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>143</v>
       </c>
@@ -4103,7 +4108,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>143</v>
       </c>
@@ -4117,7 +4122,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>143</v>
       </c>
@@ -4131,7 +4136,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
@@ -4145,7 +4150,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>143</v>
       </c>
@@ -4159,7 +4164,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
@@ -4173,7 +4178,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>143</v>
       </c>
@@ -4187,7 +4192,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>143</v>
       </c>
@@ -4201,7 +4206,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>143</v>
       </c>
@@ -4215,7 +4220,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>143</v>
       </c>
@@ -4229,7 +4234,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>143</v>
       </c>
@@ -4243,7 +4248,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>143</v>
       </c>
@@ -4257,7 +4262,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>143</v>
       </c>
@@ -4271,7 +4276,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
@@ -4285,7 +4290,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>143</v>
       </c>
@@ -4299,7 +4304,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>143</v>
       </c>
@@ -4313,7 +4318,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>143</v>
       </c>
@@ -4327,7 +4332,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>143</v>
       </c>
@@ -4341,7 +4346,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>143</v>
       </c>
@@ -4355,7 +4360,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>143</v>
       </c>
@@ -4369,7 +4374,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>143</v>
       </c>
@@ -4383,7 +4388,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>143</v>
       </c>
@@ -4397,7 +4402,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>143</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
@@ -4425,7 +4430,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -4439,7 +4444,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>143</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>143</v>
       </c>
@@ -4467,7 +4472,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>143</v>
       </c>
@@ -4481,7 +4486,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>143</v>
       </c>
@@ -4495,7 +4500,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>143</v>
       </c>
@@ -4509,7 +4514,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>143</v>
       </c>
@@ -4523,7 +4528,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>143</v>
       </c>
@@ -4537,7 +4542,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>143</v>
       </c>
@@ -4551,7 +4556,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>143</v>
       </c>
@@ -4565,7 +4570,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>143</v>
       </c>
@@ -4579,7 +4584,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>143</v>
       </c>
@@ -4593,7 +4598,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -4607,7 +4612,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>143</v>
       </c>
@@ -4621,7 +4626,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>143</v>
       </c>
@@ -4635,7 +4640,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>143</v>
       </c>
@@ -4649,7 +4654,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>143</v>
       </c>
@@ -4663,7 +4668,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>143</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -4691,7 +4696,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>99</v>
       </c>
@@ -4705,7 +4710,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>99</v>
       </c>
@@ -4719,7 +4724,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>99</v>
       </c>
@@ -4733,7 +4738,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>102</v>
       </c>
@@ -4747,7 +4752,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>102</v>
       </c>
@@ -4761,7 +4766,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>102</v>
       </c>
@@ -4775,7 +4780,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>69</v>
       </c>
@@ -4789,7 +4794,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>69</v>
       </c>
@@ -4803,7 +4808,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
@@ -4817,7 +4822,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>69</v>
       </c>
@@ -4831,7 +4836,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>91</v>
       </c>
@@ -4845,7 +4850,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>91</v>
       </c>
@@ -4859,7 +4864,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>91</v>
       </c>
@@ -4873,7 +4878,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>91</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>91</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>91</v>
       </c>
@@ -4915,7 +4920,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>91</v>
       </c>
@@ -4929,7 +4934,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>91</v>
       </c>
@@ -4943,7 +4948,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>91</v>
       </c>
@@ -4957,7 +4962,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
@@ -4971,7 +4976,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
@@ -4985,7 +4990,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>91</v>
       </c>
@@ -4999,7 +5004,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -5013,7 +5018,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -5027,7 +5032,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>196</v>
       </c>
@@ -5041,7 +5046,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>196</v>
       </c>
@@ -5055,7 +5060,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>196</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>196</v>
       </c>
@@ -5083,7 +5088,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>196</v>
       </c>
@@ -5097,7 +5102,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>196</v>
       </c>
@@ -5111,7 +5116,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>196</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>196</v>
       </c>
@@ -5139,7 +5144,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>201</v>
       </c>
@@ -5153,7 +5158,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>185</v>
       </c>
@@ -5167,7 +5172,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>185</v>
       </c>
@@ -5181,7 +5186,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>421</v>
       </c>
@@ -5195,7 +5200,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>421</v>
       </c>
@@ -5209,7 +5214,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>421</v>
       </c>
@@ -5237,15 +5242,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>215</v>
       </c>
@@ -5259,7 +5264,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5273,7 +5278,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -5301,7 +5306,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5315,7 +5320,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -5329,7 +5334,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -5343,7 +5348,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5357,7 +5362,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -5371,7 +5376,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -5385,7 +5390,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -5399,7 +5404,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -5441,7 +5446,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -5455,7 +5460,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -5469,7 +5474,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -5483,7 +5488,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -5497,7 +5502,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -5511,7 +5516,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -5539,7 +5544,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -5553,7 +5558,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -5581,7 +5586,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -5595,7 +5600,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -5609,7 +5614,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
@@ -5623,7 +5628,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -5651,7 +5656,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -5665,7 +5670,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -5679,7 +5684,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -5693,7 +5698,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -5707,7 +5712,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -5721,7 +5726,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -5735,7 +5740,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -5749,7 +5754,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -5763,7 +5768,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
@@ -5777,7 +5782,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
@@ -5791,7 +5796,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
@@ -5805,7 +5810,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>69</v>
       </c>
@@ -5819,7 +5824,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>69</v>
       </c>
@@ -5833,7 +5838,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -5847,7 +5852,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -5861,7 +5866,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -5875,7 +5880,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>77</v>
       </c>
@@ -5889,7 +5894,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
@@ -5903,7 +5908,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>82</v>
       </c>
@@ -5917,7 +5922,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>82</v>
       </c>
@@ -5931,7 +5936,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>82</v>
       </c>
@@ -5945,7 +5950,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>82</v>
       </c>
@@ -5959,7 +5964,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>91</v>
       </c>
@@ -5973,7 +5978,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>91</v>
       </c>
@@ -5987,7 +5992,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
@@ -6001,7 +6006,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>91</v>
       </c>
@@ -6015,7 +6020,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>91</v>
       </c>
@@ -6029,7 +6034,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>91</v>
       </c>
@@ -6043,7 +6048,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>91</v>
       </c>
@@ -6057,7 +6062,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>91</v>
       </c>
@@ -6071,7 +6076,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>91</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>91</v>
       </c>
@@ -6099,7 +6104,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>91</v>
       </c>
@@ -6113,7 +6118,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>91</v>
       </c>
@@ -6127,7 +6132,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>91</v>
       </c>
@@ -6141,7 +6146,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>91</v>
       </c>
@@ -6155,7 +6160,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>91</v>
       </c>
@@ -6169,7 +6174,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>94</v>
       </c>
@@ -6183,7 +6188,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>94</v>
       </c>
@@ -6197,7 +6202,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>99</v>
       </c>
@@ -6211,7 +6216,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>99</v>
       </c>
@@ -6225,7 +6230,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>99</v>
       </c>
@@ -6239,7 +6244,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>99</v>
       </c>
@@ -6253,7 +6258,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>102</v>
       </c>
@@ -6267,7 +6272,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>102</v>
       </c>
@@ -6281,7 +6286,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>102</v>
       </c>
@@ -6295,7 +6300,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>102</v>
       </c>
@@ -6309,7 +6314,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>105</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>105</v>
       </c>
@@ -6337,7 +6342,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>105</v>
       </c>
@@ -6351,7 +6356,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>105</v>
       </c>
@@ -6365,7 +6370,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>105</v>
       </c>
@@ -6379,7 +6384,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>116</v>
       </c>
@@ -6393,7 +6398,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>119</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>119</v>
       </c>
@@ -6421,7 +6426,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>122</v>
       </c>
@@ -6435,7 +6440,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>105</v>
       </c>
@@ -6449,7 +6454,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>105</v>
       </c>
@@ -6463,7 +6468,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>105</v>
       </c>
@@ -6477,7 +6482,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>105</v>
       </c>
@@ -6491,7 +6496,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>105</v>
       </c>
@@ -6505,7 +6510,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>105</v>
       </c>
@@ -6519,7 +6524,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>105</v>
       </c>
@@ -6533,7 +6538,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>105</v>
       </c>
@@ -6547,7 +6552,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>105</v>
       </c>
@@ -6561,7 +6566,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>143</v>
       </c>
@@ -6575,7 +6580,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>143</v>
       </c>
@@ -6589,7 +6594,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>143</v>
       </c>
@@ -6603,7 +6608,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>143</v>
       </c>
@@ -6617,7 +6622,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>143</v>
       </c>
@@ -6631,7 +6636,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>143</v>
       </c>
@@ -6645,7 +6650,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>143</v>
       </c>
@@ -6659,7 +6664,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>143</v>
       </c>
@@ -6673,7 +6678,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>143</v>
       </c>
@@ -6687,7 +6692,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>143</v>
       </c>
@@ -6701,7 +6706,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>143</v>
       </c>
@@ -6715,7 +6720,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>143</v>
       </c>
@@ -6729,7 +6734,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>143</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>143</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>143</v>
       </c>
@@ -6771,7 +6776,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>143</v>
       </c>
@@ -6785,7 +6790,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>143</v>
       </c>
@@ -6799,7 +6804,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>143</v>
       </c>
@@ -6813,7 +6818,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>143</v>
       </c>
@@ -6827,7 +6832,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>143</v>
       </c>
@@ -6841,7 +6846,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>143</v>
       </c>
@@ -6855,7 +6860,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>143</v>
       </c>
@@ -6869,7 +6874,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>143</v>
       </c>
@@ -6883,7 +6888,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>143</v>
       </c>
@@ -6897,7 +6902,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>143</v>
       </c>
@@ -6911,7 +6916,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>143</v>
       </c>
@@ -6925,7 +6930,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>143</v>
       </c>
@@ -6939,7 +6944,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>143</v>
       </c>
@@ -6953,7 +6958,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>143</v>
       </c>
@@ -6967,7 +6972,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>143</v>
       </c>
@@ -6981,7 +6986,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>143</v>
       </c>
@@ -6995,7 +7000,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>143</v>
       </c>
@@ -7009,7 +7014,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>143</v>
       </c>
@@ -7023,7 +7028,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>143</v>
       </c>
@@ -7037,7 +7042,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>143</v>
       </c>
@@ -7051,7 +7056,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>143</v>
       </c>
@@ -7065,7 +7070,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>143</v>
       </c>
@@ -7079,7 +7084,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>143</v>
       </c>
@@ -7093,7 +7098,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>143</v>
       </c>
@@ -7107,7 +7112,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>143</v>
       </c>
@@ -7121,7 +7126,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>143</v>
       </c>
@@ -7135,7 +7140,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>143</v>
       </c>
@@ -7149,7 +7154,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>143</v>
       </c>
@@ -7163,7 +7168,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>143</v>
       </c>
@@ -7177,7 +7182,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>143</v>
       </c>
@@ -7191,7 +7196,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>143</v>
       </c>
@@ -7205,7 +7210,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>143</v>
       </c>
@@ -7219,7 +7224,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>143</v>
       </c>
@@ -7233,7 +7238,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>143</v>
       </c>
@@ -7247,7 +7252,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
@@ -7261,7 +7266,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>143</v>
       </c>
@@ -7275,7 +7280,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>143</v>
       </c>
@@ -7289,7 +7294,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>143</v>
       </c>
@@ -7303,7 +7308,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>143</v>
       </c>
@@ -7317,7 +7322,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>143</v>
       </c>
@@ -7331,7 +7336,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>143</v>
       </c>
@@ -7345,7 +7350,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>143</v>
       </c>
@@ -7359,7 +7364,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>143</v>
       </c>
@@ -7373,7 +7378,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>143</v>
       </c>
@@ -7387,7 +7392,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>143</v>
       </c>
@@ -7401,7 +7406,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>158</v>
       </c>
@@ -7415,7 +7420,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>161</v>
       </c>
@@ -7429,7 +7434,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>164</v>
       </c>
@@ -7443,7 +7448,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>164</v>
       </c>
@@ -7457,7 +7462,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>164</v>
       </c>
@@ -7471,7 +7476,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>164</v>
       </c>
@@ -7485,7 +7490,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>164</v>
       </c>
@@ -7499,7 +7504,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>164</v>
       </c>
@@ -7513,7 +7518,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>164</v>
       </c>
@@ -7527,7 +7532,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>164</v>
       </c>
@@ -7541,7 +7546,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
@@ -7555,7 +7560,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>164</v>
       </c>
@@ -7569,7 +7574,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>185</v>
       </c>
@@ -7583,7 +7588,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>185</v>
       </c>
@@ -7597,7 +7602,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>185</v>
       </c>
@@ -7611,7 +7616,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>188</v>
       </c>
@@ -7625,7 +7630,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>188</v>
       </c>
@@ -7639,7 +7644,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>188</v>
       </c>
@@ -7653,7 +7658,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>188</v>
       </c>
@@ -7667,7 +7672,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>191</v>
       </c>
@@ -7681,7 +7686,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>193</v>
       </c>
@@ -7695,7 +7700,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>193</v>
       </c>
@@ -7709,7 +7714,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>193</v>
       </c>
@@ -7723,7 +7728,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>193</v>
       </c>
@@ -7737,7 +7742,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>193</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>193</v>
       </c>
@@ -7765,7 +7770,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>196</v>
       </c>
@@ -7779,7 +7784,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>196</v>
       </c>
@@ -7793,7 +7798,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>196</v>
       </c>
@@ -7807,7 +7812,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>196</v>
       </c>
@@ -7821,7 +7826,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>196</v>
       </c>
@@ -7835,7 +7840,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>196</v>
       </c>
@@ -7849,7 +7854,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>196</v>
       </c>
@@ -7863,7 +7868,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>196</v>
       </c>
@@ -7877,7 +7882,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>196</v>
       </c>
@@ -7891,7 +7896,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>196</v>
       </c>
@@ -7905,7 +7910,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>196</v>
       </c>
@@ -7919,7 +7924,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>201</v>
       </c>
@@ -7933,7 +7938,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>201</v>
       </c>
@@ -7947,7 +7952,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>204</v>
       </c>
@@ -7961,7 +7966,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>204</v>
       </c>
@@ -7975,7 +7980,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>421</v>
       </c>
@@ -7989,7 +7994,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>421</v>
       </c>
@@ -8003,7 +8008,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>421</v>
       </c>
@@ -8017,7 +8022,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>209</v>
       </c>
@@ -8039,6 +8044,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8152,22 +8172,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31F5E297-07EC-486E-A691-9ACD12C364A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8181,27 +8209,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31F5E297-07EC-486E-A691-9ACD12C364A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>